<commit_message>
add Create Category page
</commit_message>
<xml_diff>
--- a/src/test/resources/grocela_Admin_Portal.xlsx
+++ b/src/test/resources/grocela_Admin_Portal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ANIL TASK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\eclipse-workspace\GROCELA_Admin_Portal\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{936FCB2F-BB68-4FA6-9BCF-AD102355976E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2075AA-5A86-4273-9273-8450D31E3D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{CB53A64C-0502-4751-92CE-87921612D9CA}"/>
   </bookViews>
@@ -25,7 +25,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Category name</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Fruits are nature's delicious and nutritious gifts They come in a variety of flavors, textures, and colors, offering essential vitamins, minerals, and fiber. Here are</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegetables are packed with nutrients and offer countless health benefits They come in many varieties, each bringing unique flavors, textures, and nutritional 
+</t>
+  </si>
   <si>
     <t>SL NO</t>
   </si>
@@ -37,13 +56,22 @@
   </si>
   <si>
     <t>tail_sub</t>
+  </si>
+  <si>
+    <t>SLNo</t>
+  </si>
+  <si>
+    <t>Home Page Banners</t>
+  </si>
+  <si>
+    <t>Create Category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,16 +79,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -83,16 +143,183 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -409,200 +636,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC62C7C-875A-4AD1-810B-1A337AFF7996}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" style="1" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11">
+        <v>5</v>
+      </c>
+      <c r="G2" s="11">
+        <v>6</v>
+      </c>
+      <c r="H2" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A6:H6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>